<commit_message>
created the bot as 1 sequence
</commit_message>
<xml_diff>
--- a/InvoiceBot/InvoiceDataLog.xlsx
+++ b/InvoiceBot/InvoiceDataLog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubProjects\INVOICEProcessingfBot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubProjects\New InvoiceProcessing\InvoiceBot2\InvoiceBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FDE4A3-D343-49E8-B4E0-CA0F117145A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE2722E-BA1F-4DB3-8D19-F3EC527BC3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{71BB526B-92F3-4D18-935F-43566BE0BC34}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{71BB526B-92F3-4D18-935F-43566BE0BC34}"/>
   </bookViews>
   <sheets>
     <sheet name="InvoiceLog" sheetId="1" r:id="rId1"/>
@@ -147,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -156,9 +156,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -257,8 +254,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}" name="Table1" displayName="Table1" ref="A1:X19" totalsRowShown="0">
-  <autoFilter ref="A1:X19" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}" name="Table1" displayName="Table1" ref="A1:X18" totalsRowShown="0">
+  <autoFilter ref="A1:X18" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}"/>
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{0FA06E5B-1B73-4E73-A44D-1DA293421287}" name="#NO" dataDxfId="23">
       <calculatedColumnFormula>ROW()-1</calculatedColumnFormula>
@@ -608,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B17B189-3F58-460C-B125-67DE3543A8D8}">
-  <dimension ref="A1:X19"/>
+  <dimension ref="A1:X18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -707,10 +704,10 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <f t="shared" ref="A2:A19" si="0">ROW()-1</f>
+        <f t="shared" ref="A2:A18" si="0">ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1198,35 +1195,6 @@
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="3"/>
-      <c r="X19" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
made description a multi-value
</commit_message>
<xml_diff>
--- a/InvoiceBot/InvoiceDataLog.xlsx
+++ b/InvoiceBot/InvoiceDataLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubProjects\New InvoiceProcessing\InvoiceBot2\InvoiceBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE2722E-BA1F-4DB3-8D19-F3EC527BC3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68681DA3-88E4-420D-88A7-32F35F23F478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{71BB526B-92F3-4D18-935F-43566BE0BC34}"/>
+    <workbookView xWindow="31650" yWindow="3225" windowWidth="17280" windowHeight="8880" xr2:uid="{71BB526B-92F3-4D18-935F-43566BE0BC34}"/>
   </bookViews>
   <sheets>
     <sheet name="InvoiceLog" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>#NO</t>
   </si>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>V.I.B. Bookshop CC</t>
+  </si>
+  <si>
+    <t>UNC</t>
+  </si>
+  <si>
+    <t>U.W.C. Student Centre Modderdam Road, Bellville 7500 PO Box 278, Kasselvlei 7533</t>
+  </si>
+  <si>
+    <t>ROBERT SORUKNE RD BEUVLUG 7535</t>
   </si>
 </sst>
 </file>
@@ -147,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -156,6 +168,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -707,14 +722,28 @@
         <f t="shared" ref="A2:A18" si="0">ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="B2" s="4">
+        <v>45238</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="H2" s="1">
+        <v>8365</v>
+      </c>
+      <c r="I2" s="1">
+        <v>4100222985</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>

</xml_diff>

<commit_message>
deleted previous data off excel
</commit_message>
<xml_diff>
--- a/InvoiceBot/InvoiceDataLog.xlsx
+++ b/InvoiceBot/InvoiceDataLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubProjects\New InvoiceProcessing\InvoiceBot2\InvoiceBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68681DA3-88E4-420D-88A7-32F35F23F478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41006736-4F43-4405-9219-472B3D0EF57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31650" yWindow="3225" windowWidth="17280" windowHeight="8880" xr2:uid="{71BB526B-92F3-4D18-935F-43566BE0BC34}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{71BB526B-92F3-4D18-935F-43566BE0BC34}"/>
   </bookViews>
   <sheets>
     <sheet name="InvoiceLog" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>#NO</t>
   </si>
@@ -108,18 +108,6 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>V.I.B. Bookshop CC</t>
-  </si>
-  <si>
-    <t>UNC</t>
-  </si>
-  <si>
-    <t>U.W.C. Student Centre Modderdam Road, Bellville 7500 PO Box 278, Kasselvlei 7533</t>
-  </si>
-  <si>
-    <t>ROBERT SORUKNE RD BEUVLUG 7535</t>
   </si>
 </sst>
 </file>
@@ -159,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -168,9 +156,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -269,8 +254,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}" name="Table1" displayName="Table1" ref="A1:X18" totalsRowShown="0">
-  <autoFilter ref="A1:X18" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}" name="Table1" displayName="Table1" ref="A1:X17" totalsRowShown="0">
+  <autoFilter ref="A1:X17" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}"/>
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{0FA06E5B-1B73-4E73-A44D-1DA293421287}" name="#NO" dataDxfId="23">
       <calculatedColumnFormula>ROW()-1</calculatedColumnFormula>
@@ -620,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B17B189-3F58-460C-B125-67DE3543A8D8}">
-  <dimension ref="A1:X18"/>
+  <dimension ref="A1:X17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H2"/>
+      <selection activeCell="B2" sqref="B2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -719,31 +704,17 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <f t="shared" ref="A2:A18" si="0">ROW()-1</f>
+        <f t="shared" ref="A2:A17" si="0">ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="4">
-        <v>45238</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="1">
-        <v>8365</v>
-      </c>
-      <c r="I2" s="1">
-        <v>4100222985</v>
-      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -1195,35 +1166,6 @@
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
added export merge to loop
</commit_message>
<xml_diff>
--- a/InvoiceBot/InvoiceDataLog.xlsx
+++ b/InvoiceBot/InvoiceDataLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubProjects\New InvoiceProcessing\InvoiceBot2\InvoiceBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41006736-4F43-4405-9219-472B3D0EF57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C4288A-3702-491D-87E8-F815ED2DCB76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{71BB526B-92F3-4D18-935F-43566BE0BC34}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{71BB526B-92F3-4D18-935F-43566BE0BC34}"/>
   </bookViews>
   <sheets>
     <sheet name="InvoiceLog" sheetId="1" r:id="rId1"/>
@@ -254,8 +254,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}" name="Table1" displayName="Table1" ref="A1:X17" totalsRowShown="0">
-  <autoFilter ref="A1:X17" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}" name="Table1" displayName="Table1" ref="A1:X22" totalsRowShown="0">
+  <autoFilter ref="A1:X22" xr:uid="{CDCB10E2-29B8-4D55-8CF7-8C0CEA953F15}"/>
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{0FA06E5B-1B73-4E73-A44D-1DA293421287}" name="#NO" dataDxfId="23">
       <calculatedColumnFormula>ROW()-1</calculatedColumnFormula>
@@ -605,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B17B189-3F58-460C-B125-67DE3543A8D8}">
-  <dimension ref="A1:X17"/>
+  <dimension ref="A1:X22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I2"/>
+      <selection activeCell="A2" sqref="A2:X22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -621,7 +621,8 @@
     <col min="10" max="12" width="30.77734375" customWidth="1"/>
     <col min="13" max="13" width="182.6640625" customWidth="1"/>
     <col min="14" max="17" width="30.77734375" customWidth="1"/>
-    <col min="18" max="19" width="104" customWidth="1"/>
+    <col min="18" max="18" width="104" customWidth="1"/>
+    <col min="19" max="19" width="71.44140625" customWidth="1"/>
     <col min="20" max="20" width="43.44140625" customWidth="1"/>
     <col min="21" max="21" width="30.77734375" customWidth="1"/>
     <col min="22" max="22" width="39.6640625" customWidth="1"/>
@@ -704,7 +705,7 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <f t="shared" ref="A2:A17" si="0">ROW()-1</f>
+        <f t="shared" ref="A2:A22" si="0">ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" s="1"/>
@@ -1166,6 +1167,151 @@
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
     </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>